<commit_message>
Modificación leve de Excel con data útil.
</commit_message>
<xml_diff>
--- a/database/DB y Operaciones de Usuario.xlsx
+++ b/database/DB y Operaciones de Usuario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes Draft" sheetId="1" r:id="rId1"/>
@@ -7920,8 +7920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9843,8 +9843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D50"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hojas de Firmas de Catedráticos
</commit_message>
<xml_diff>
--- a/database/DB y Operaciones de Usuario.xlsx
+++ b/database/DB y Operaciones de Usuario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes Draft" sheetId="1" r:id="rId1"/>
@@ -7920,8 +7920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB90"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9843,7 +9843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Nuevo diagrama entidad relación y rollback entre los queries prueba
</commit_message>
<xml_diff>
--- a/database/DB y Operaciones de Usuario.xlsx
+++ b/database/DB y Operaciones de Usuario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="224">
   <si>
     <t>Teléfonos</t>
   </si>
@@ -735,30 +735,15 @@
     <t>Especificar este constraint.</t>
   </si>
   <si>
-    <t>id_address: int(11)</t>
-  </si>
-  <si>
     <t>address: varchar(140)</t>
   </si>
   <si>
     <t>id_correspondiente: int(11)</t>
   </si>
   <si>
-    <t>id_asesor: int(11) - Auto-Increment</t>
-  </si>
-  <si>
-    <t>id_postulante: int(11) - Auto-Increment</t>
-  </si>
-  <si>
-    <t>id_empleado: int(11) - Auto-Increment</t>
-  </si>
-  <si>
     <t>id_catedratico: int(11) - Auto-Increment</t>
   </si>
   <si>
-    <t>id_asignacion_catedratico: int(11) - Auto-Increment</t>
-  </si>
-  <si>
     <t>Empleado_Laborando</t>
   </si>
   <si>
@@ -769,6 +754,24 @@
   </si>
   <si>
     <t>*id_sistema: int(11)</t>
+  </si>
+  <si>
+    <t>id_address: int(11), Auto_Increment</t>
+  </si>
+  <si>
+    <t>id_asesor: int(11), Auto_Increment</t>
+  </si>
+  <si>
+    <t>id_postulante: int(11), Auto_Increment</t>
+  </si>
+  <si>
+    <t>id_empleado: int(11), Auto_Increment</t>
+  </si>
+  <si>
+    <t>id_asignacion_catedratico: int(11), Auto_Increment</t>
+  </si>
+  <si>
+    <t>(1,1)</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1469,8 +1472,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3451,6 +3460,138 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>461596</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>464635</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Conector recto 45"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8447942" y="1157654"/>
+          <a:ext cx="3039" cy="2403231"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>460346</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>83098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1788</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>94714</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Conector recto 49"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8446692" y="3556060"/>
+          <a:ext cx="8326423" cy="11616"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>915865</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Conector recto 52"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16764000" y="3568212"/>
+          <a:ext cx="359019" cy="864576"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -4155,8 +4296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,17 +4314,17 @@
     <col min="14" max="14" width="12.85546875" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
     <col min="19" max="19" width="5.28515625" customWidth="1"/>
     <col min="20" max="20" width="18.42578125" customWidth="1"/>
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="12.5703125" customWidth="1"/>
     <col min="23" max="23" width="16.140625" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
     <col min="25" max="25" width="16.28515625" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="27" max="27" width="28" customWidth="1"/>
     <col min="28" max="28" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4228,10 +4369,10 @@
       <c r="AA3" s="61"/>
     </row>
     <row r="4" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="J4" s="62" t="s">
-        <v>220</v>
-      </c>
-      <c r="K4" s="12"/>
+      <c r="J4" s="110" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="138"/>
       <c r="L4" s="12"/>
       <c r="M4" s="15" t="s">
         <v>17</v>
@@ -4240,7 +4381,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="23" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R4" s="16"/>
       <c r="S4" s="48"/>
@@ -4255,10 +4396,10 @@
       <c r="AA4" s="63"/>
     </row>
     <row r="5" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="J5" s="138" t="s">
-        <v>222</v>
-      </c>
-      <c r="K5" s="139"/>
+      <c r="J5" s="139" t="s">
+        <v>217</v>
+      </c>
+      <c r="K5" s="140"/>
       <c r="L5" s="12"/>
       <c r="M5" s="17" t="s">
         <v>206</v>
@@ -4267,7 +4408,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R5" s="18"/>
       <c r="S5" s="48"/>
@@ -4284,10 +4425,10 @@
       <c r="AA5" s="63"/>
     </row>
     <row r="6" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="J6" s="138" t="s">
-        <v>221</v>
-      </c>
-      <c r="K6" s="139"/>
+      <c r="J6" s="141" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="142"/>
       <c r="L6" s="12"/>
       <c r="M6" s="17" t="s">
         <v>18</v>
@@ -4311,7 +4452,9 @@
       <c r="AA6" s="63"/>
     </row>
     <row r="7" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="J7" s="62"/>
+      <c r="J7" s="143" t="s">
+        <v>223</v>
+      </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="56" t="s">
@@ -4415,7 +4558,7 @@
     <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="J11" s="62"/>
       <c r="K11" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="12"/>
@@ -4672,7 +4815,7 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
       <c r="T20" s="99" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="U20" s="101"/>
       <c r="V20" s="12"/>
@@ -4709,20 +4852,20 @@
       <c r="M21" s="63"/>
       <c r="O21" s="62"/>
       <c r="P21" s="53" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="Q21" s="16"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="53" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="U21" s="16"/>
       <c r="V21" s="12" t="s">
         <v>117</v>
       </c>
       <c r="W21" s="53" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="X21" s="16"/>
       <c r="Y21" s="12"/>
@@ -4845,7 +4988,9 @@
       </c>
       <c r="Q24" s="18"/>
       <c r="R24" s="12"/>
-      <c r="S24" s="12"/>
+      <c r="S24" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="T24" s="17" t="s">
         <v>22</v>
       </c>
@@ -4930,7 +5075,7 @@
         <v>71</v>
       </c>
       <c r="W26" s="53" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="X26" s="16"/>
       <c r="Y26" s="12" t="s">
@@ -5027,7 +5172,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="Z28" s="53" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AA28" s="16"/>
       <c r="AB28" s="63"/>

</xml_diff>